<commit_message>
Maj Doc + Cartons rouges dans calcul cartons jaunes
</commit_message>
<xml_diff>
--- a/Analyse/Liste Règles contrôles.xlsx
+++ b/Analyse/Liste Règles contrôles.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Personnel - OH\Divers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivier\Desktop\Projets Git\FifaManagerEphec\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0457D46A-3B80-4F63-AF10-718388B0A43F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="242">
   <si>
     <t>R1</t>
   </si>
@@ -687,12 +689,273 @@
   <si>
     <t>Feuille de match</t>
   </si>
+  <si>
+    <t>BDD : Contrainte not null</t>
+  </si>
+  <si>
+    <t>Numéro+F33C2A1:E23A1:F44C2A1:F48</t>
+  </si>
+  <si>
+    <t>BDD : Contrainte not null
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : Contrainte unique
+BDD : BackEnd.Championnat_Add (PS)
+BL : ChampionnatsService
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : FormatAnneesChampionnats (Trigger)
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : Contrainte unique
+BDD : BackEnd.Intersaisons.Add (PS)
+BDD : Intersaisons_UniciteChampionnat (Trigger)
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Intersaisons.Add (PS)
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Quarters.Add (PS)
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Quarters.Add  (PS)
+BDD : MaxQuarters (Trigger)
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : Contrainte unique
+BDD : Equipes_UniciteNom (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD : Valeur par défaut noLogo</t>
+  </si>
+  <si>
+    <t>BDD : Contrainte unique equipeId / championnatId
+BDD : BackEnd.EquipeParticipation_Add (PS)
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.EquipeParticipation_Add (PS)
+BDD : EquipesParticipation_EquipeActive (Trigger)
+BL : GenerationTabEquipeSelection
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BL : GenerationTabEquipeSelection
+FORM : Générer un championnat</t>
+  </si>
+  <si>
+    <t>BDD : Valeur par défaut 0</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Matchs_Add (PS)
+BDD : BackEnd et MatchManagement.Matchs_Update (PS)
+BDD : Matchs_WithinChampionnat (Trigger)
+BL : GenerationTabCalendrierMatchs
+FORM : Calendrier des matchs</t>
+  </si>
+  <si>
+    <t>Où ?</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Matchs_Add (PS)
+BDD : BackEnd et MatchManagement.Matchs_Update (PS)
+BDD : Matchs_SameTeams  (Trigger)
+BL : GenerationTabCalendrierMatchs
+FORM : Calendrier des matchs</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Matchs_Add (PS)
+BDD : BackEnd et MatchManagement.Matchs_Update (PS)
+BDD : Matchs_Doublons   (Trigger)
+BL : GenerationTabCalendrierMatchs
+FORM : Calendrier des matchs</t>
+  </si>
+  <si>
+    <t>BL : GenerationTabCalendrierMatchs
+FORM : Calendrier des matchs</t>
+  </si>
+  <si>
+    <t>BDD : Matchs_UpdatePlusVieux (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD : CartonsJaunesHistory_PlayedMatch (Trigger)
+BL : CartesJaunesService</t>
+  </si>
+  <si>
+    <t>BDD : CartonsRougesHistory_PlayedMatch (Trigger)
+BL : CartesRougesService</t>
+  </si>
+  <si>
+    <t>BDD : GoalsHistory_PlayedMatch (Trigger)
+BL : GoalsService</t>
+  </si>
+  <si>
+    <t>Si une des 2 feuilles de match compte moins de 5 joueurs alors le match est considéré comme joué</t>
+  </si>
+  <si>
+    <t>BL : CheckConditionsResultats</t>
+  </si>
+  <si>
+    <t>BDD : JoueursParticipationHistory_CheckFeuillesDeMatch (Trigger)
+FORM : Feuille de match</t>
+  </si>
+  <si>
+    <t>BL : GenerationTableauxFeuille
+FORM : Feuille de Match
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD: CartonsRougesHistory_EstDansFeuilleDeMatch (Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD : CartonsRougesHistory_UpdatePlusVieux (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD : CartonsJaunesHistory_LimiteMinuteRecue  (Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD : MatchManagement.CartonsRougesHistory_Add (PS)
+BDD : MatchManagement.CartonsRouges_Update (PS)
+BDD : CartonsRougesHistory_MaxCartonParMatch (Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD : CartonsJaunesHistory_UpdatePlusVieux (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD : CartonsJaunesHistory_EstDansFeuilleDeMatch(Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD : Valeur par défaut isActive 1</t>
+  </si>
+  <si>
+    <t>BDD : GoalsHistory_LimiteMinuteRecue (Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD: CartonsRougesHistory_LimiteMinuteRecue (Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD : GoalsHistory_UpdatePlusVieux (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD: GoalsHistory_EstDansFeuilleDeMatch  (Trigger)
+FORM : Inscriptions des résultats</t>
+  </si>
+  <si>
+    <t>BDD : CartonsRougesHistory_EnoughJoueurs (Trigger)
+BL : CheckConditionsResultats
+FORM : Accueil MatchManagement, Inscription des résultats</t>
+  </si>
+  <si>
+    <t>BDD : CartonsJaunesHistory_EnoughJoueurs  (Trigger)
+BL : CheckConditionsResultats
+FORM : Accueil MatchManagement, Inscription des résultats</t>
+  </si>
+  <si>
+    <t>BDD : GoalsHistory_EnoughJoueurs (Trigger)
+BL : CheckConditionsResultats
+FORM : Accueil MatchManagement, Inscription des résultats</t>
+  </si>
+  <si>
+    <t>Il ne peut y avoir qu’une feuille de match pour une équipe pour un match précis.</t>
+  </si>
+  <si>
+    <t>Un goal ne peut être marqué que par un joueur qui joue le match</t>
+  </si>
+  <si>
+    <t>BDD : MatchManagement.FeuilleDeMatch_Add (PS)
+BDD : MatchManagement.FeuilleDeMatch_Update (PS)
+BDD : FeuillesDeMatch_MaxFeuilleParEquipe (Trigger)
+BL : FeuillesMatchService</t>
+  </si>
+  <si>
+    <t>BDD : MatchManagement.FeuilleDeMatch_Add (PS)
+BDD : MatchManagement.FeuilleDeMatch_Update (PS)
+BDD : FeuillesDeMatch_MaxFeuilleParMatch  (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD : MatchManagement.FeuilleDeMatch_Update (PS)
+BDD : FeuillesDeMatch_UpdatePlusVieux (Trigger)</t>
+  </si>
+  <si>
+    <t>BDD : TransfertsHistory_NombreJoueursMax (Trigger)
+BDD : TransfertsHistory_NombreJoueurs (Trigger)
+BL : TransfertsService</t>
+  </si>
+  <si>
+    <t>BDD : TransfertsHistory_DateTransfert (Trigger)
+BL : TransfertsService</t>
+  </si>
+  <si>
+    <t>Aucun transfert ne peut avoir lieu si une des 2 équipes a encore des matchs à jouer à une date ultérieure (dans les limites du championnat)</t>
+  </si>
+  <si>
+    <t>BL : TransfertsService</t>
+  </si>
+  <si>
+    <t>BDD : BackEnd.Tansferts_Add (PS)
+BDD : TransfertsHistory_DeuxEquipes (Trigger)
+BL : TransfertsService</t>
+  </si>
+  <si>
+    <t>BDD : TransfertsHistory_UpdatePlusVieux (Trigger)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDD : MatchManagement.JoueursParticipation_Add (PS)
+BDD : JoueursParticipationHistory_Max (Trigger)
+BDD : JoueursParFeuille (Trigger)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDD : MatchManagement.JoueursParticipation_Add (PS)
+BDD : JoueursParticipationHistory_EstDansEquipe (Trigger)
+FORM : Feuille de match
+</t>
+  </si>
+  <si>
+    <t>BDD : MatchManagement.JoueursParticipation_Add (PS)
+BDD : JoueursParticipationHistory_CartonRouge (Trigger)
+FORM : Feuille de match</t>
+  </si>
+  <si>
+    <t>BL : GenerationTableauxFeuille</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>Une feuille de match ne peut être remplie que si les antérieure l'on également été.</t>
+  </si>
+  <si>
+    <t>FORM : Accueil MatchManagement</t>
+  </si>
+  <si>
+    <t>Pour qu'un goal soit inscrit ou modifié, il faut qu'il n'y ait pas eu de transferts postérieurs (dans un même championnat)</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -729,6 +992,17 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -810,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -852,24 +1126,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="9.5"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -915,6 +1208,41 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
       </border>
     </dxf>
     <dxf>
@@ -1073,10 +1401,101 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1093,15 +1512,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F57" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" tableBorderDxfId="8">
-  <autoFilter ref="A1:F57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau2" displayName="Tableau2" ref="A1:F57" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:F57" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Numéro" dataDxfId="0"/>
-    <tableColumn id="2" name="Règle" dataDxfId="1"/>
-    <tableColumn id="3" name="BDD" dataDxfId="7"/>
-    <tableColumn id="4" name="Procédure stockée" dataDxfId="6"/>
-    <tableColumn id="5" name="Trigger" dataDxfId="5"/>
-    <tableColumn id="6" name="Business - Form" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Numéro+F33C2A1:E23A1:F44C2A1:F48" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Règle" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="BDD" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Procédure stockée" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Trigger" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Business - Form" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9445731B-7079-4487-9EA0-BD9123B4C1B6}" name="Tableau24" displayName="Tableau24" ref="A1:C60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C60" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D3C577E3-25C7-4F8C-B143-133349C1C42A}" name="Numéro" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D4EBA1AB-C32E-4157-BD0D-A36D5912DAFD}" name="Règle" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F3EF7CD4-8972-4808-BF2F-6978FBF5C171}" name="Où ?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1369,11 +1800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F57" sqref="A1:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1819,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>180</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>12</v>
@@ -1414,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>2</v>
+        <v>179</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2331,4 +2762,689 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F594EED2-E151-4239-A3B7-CCC57975FC1A}">
+  <dimension ref="A1:C60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>